<commit_message>
PROJECT Milestone 1: Creating basic income/expense difference calculator.
</commit_message>
<xml_diff>
--- a/Excel_Project/BUDGET_PROJECT.xlsx
+++ b/Excel_Project/BUDGET_PROJECT.xlsx
@@ -1,26 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Excel_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D4FB9-42AD-4999-B87F-88C61713A0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>BUDGET AND EXPENSE SUMMARY</t>
+  </si>
+  <si>
+    <t>TOTAL MONTHLY INCOME</t>
+  </si>
+  <si>
+    <t>TOTAL MONTHLY EXPENSE</t>
+  </si>
+  <si>
+    <t>CASH BALANCE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,29 +63,230 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Berlin Sans FB"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Bodoni MT"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Bodoni MT"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Bodoni MT"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +566,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>7606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13">
+        <f>C3-C4</f>
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel formulas section doone along with Incomes and Expenses list in Budget project.
</commit_message>
<xml_diff>
--- a/Excel_Project/BUDGET_PROJECT.xlsx
+++ b/Excel_Project/BUDGET_PROJECT.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Excel_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7D4FB9-42AD-4999-B87F-88C61713A0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32D8803-FA62-435C-9FCD-EF6A84989AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget Calc" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthyl Incomes" sheetId="2" r:id="rId2"/>
+    <sheet name="Monthly Expenses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>BUDGET AND EXPENSE SUMMARY</t>
   </si>
@@ -46,6 +48,60 @@
   </si>
   <si>
     <t>CASH BALANCE</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Estimated Amount</t>
+  </si>
+  <si>
+    <t>Income 1</t>
+  </si>
+  <si>
+    <t>Income 2</t>
+  </si>
+  <si>
+    <t>Side Hustle 1</t>
+  </si>
+  <si>
+    <t>Rent/Mortgage</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Cell phone</t>
+  </si>
+  <si>
+    <t>Groceries</t>
+  </si>
+  <si>
+    <t>Car payment</t>
+  </si>
+  <si>
+    <t>Auto repair/maintenance</t>
+  </si>
+  <si>
+    <t>Auto Insurance</t>
+  </si>
+  <si>
+    <t>Home Insurance</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Dining</t>
+  </si>
+  <si>
+    <t>Phone/Cable</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
   </si>
 </sst>
 </file>
@@ -55,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,8 +156,15 @@
       <name val="Avenir Next LT Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +183,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -252,10 +320,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,15 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -287,8 +347,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,54 +652,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
+        <f>SUM('Monthyl Incomes'!B:B)</f>
         <v>7606</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C5" s="8">
+        <f>SUM('Monthly Expenses'!B:B)</f>
         <v>5668</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-    </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="13">
-        <f>C3-C4</f>
+      <c r="C7" s="10">
+        <f>C3-C5</f>
         <v>1938</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -637,4 +715,186 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769DB53D-0AAC-4644-8617-4C476A4CF40D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E94264-42BD-47F2-AF08-57474E473BB2}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Learnt Modeling in Excel and Apply in Budget Project to Savings Goal Calculations.
</commit_message>
<xml_diff>
--- a/Excel_Project/BUDGET_PROJECT.xlsx
+++ b/Excel_Project/BUDGET_PROJECT.xlsx
@@ -8,18 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Excel_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAFB5DA-7EB4-4D43-88F7-A00A10B4864D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE79B27E-8913-4604-A037-FE8956113531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Calc" sheetId="1" r:id="rId1"/>
-    <sheet name="Savings Goal Calc" sheetId="6" r:id="rId2"/>
-    <sheet name="Monthyl Incomes" sheetId="2" r:id="rId3"/>
-    <sheet name="Monthly Expenses" sheetId="3" r:id="rId4"/>
-    <sheet name="Spending Summary" sheetId="5" r:id="rId5"/>
-    <sheet name="Transaction History" sheetId="4" r:id="rId6"/>
+    <sheet name="Monthyl Incomes" sheetId="2" r:id="rId2"/>
+    <sheet name="Monthly Expenses" sheetId="3" r:id="rId3"/>
+    <sheet name="Savings Goal Calc" sheetId="6" r:id="rId4"/>
+    <sheet name="Savings Goal Linked Cells (H)" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="Savings Goal Valid Lists (H)" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="Spending Summary" sheetId="5" r:id="rId7"/>
+    <sheet name="Transaction History" sheetId="4" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="Bdgt_Calc_Out">'Budget Calc'!$D$8</definedName>
+    <definedName name="Bgt_Without_Savngs">'Savings Goal Valid Lists (H)'!$A$2:$A$3</definedName>
+    <definedName name="Bgt_Without_Svngs_Inp">'Savings Goal Calc'!$H$10</definedName>
+    <definedName name="Cur_Svngs_Inp">'Savings Goal Calc'!$D$8</definedName>
+    <definedName name="Mnthly_Svngs_Needed_Out">'Savings Goal Calc'!$D$10</definedName>
+    <definedName name="Perc_Mnthly_Inc_Out">'Savings Goal Calc'!$D$12</definedName>
+    <definedName name="Svngs_Goal_Inp">'Savings Goal Calc'!$D$4</definedName>
+    <definedName name="Tot_Mnthly_Expns_Inp">'Budget Calc'!$D$6</definedName>
+    <definedName name="Tot_Mnthly_Inc_Inp">'Budget Calc'!$D$4</definedName>
+    <definedName name="Trgt_Svngs_Date_Inp">'Savings Goal Calc'!$D$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4694" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4702" uniqueCount="105">
   <si>
     <t>BUDGET AND EXPENSE SUMMARY</t>
   </si>
@@ -334,6 +348,27 @@
   <si>
     <t>% OF MONTHLY INCOME</t>
   </si>
+  <si>
+    <t>Deduct Savings From Budget?</t>
+  </si>
+  <si>
+    <t>Budget W/O Savings?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Budget Calculated</t>
+  </si>
+  <si>
+    <t>Savings Goal Input</t>
+  </si>
+  <si>
+    <t>Savings Target Date</t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,8 +423,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +487,18 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -432,17 +516,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -456,14 +529,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -473,15 +544,87 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -493,13 +636,22 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -508,22 +660,59 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,76 +721,111 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="10" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,6 +838,119 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="'Savings Goal Linked Cells (H)'!$A$2" horiz="1" max="100" page="10" val="53"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="'Savings Goal Linked Cells (H)'!$B$2" horiz="1" max="120" min="1" page="10" val="86"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>601980</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>838200</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2057" name="Scroll Bar 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>601980</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>838200</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Scroll Bar 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E77CB55-1F19-4111-8037-55679FB2BFBD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -882,7 +1219,7 @@
   <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,10 +1227,11 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.5546875" customWidth="1"/>
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:5" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -902,66 +1240,64 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="22"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="23">
+      <c r="C4" s="9"/>
+      <c r="D4" s="45">
         <f>SUM('Monthyl Incomes'!B:B)</f>
         <v>7606</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="41"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="23">
+      <c r="C6" s="9"/>
+      <c r="D6" s="45">
         <f>SUM('Monthly Expenses'!B:B)</f>
         <v>5668</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="41"/>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="24">
-        <f>D4-D6</f>
+      <c r="C8" s="11"/>
+      <c r="D8" s="46">
+        <f>IF(Bgt_Without_Svngs_Inp="No", (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp), (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp-Cur_Svngs_Inp))</f>
         <v>1938</v>
       </c>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="2:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+  <mergeCells count="8">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -970,11 +1306,6 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -982,116 +1313,370 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383BEB5-BBAF-43B5-BACD-CE422F08E9FE}">
-  <dimension ref="B2:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769DB53D-0AAC-4644-8617-4C476A4CF40D}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E94264-42BD-47F2-AF08-57474E473BB2}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383BEB5-BBAF-43B5-BACD-CE422F08E9FE}">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="36"/>
+    </row>
+    <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="23">
-        <v>59000</v>
-      </c>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="50">
+        <f>'Savings Goal Linked Cells (H)'!A2*1000</f>
+        <v>53000</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="21"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="26">
-        <v>46926</v>
-      </c>
-      <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="51">
+        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())+'Savings Goal Linked Cells (H)'!B2, DAY(TODAY()))</f>
+        <v>47208</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" s="22"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B8" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="23">
+      <c r="C8" s="9"/>
+      <c r="D8" s="49">
         <v>3750</v>
       </c>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="20" t="s">
+      <c r="E8" s="49"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B9" s="23"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="24">
-        <f ca="1">(D4-D8)/DATEDIF(TODAY(), D6, "M")</f>
-        <v>726.97368421052636</v>
-      </c>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="20" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="47">
+        <f ca="1">(Svngs_Goal_Inp-Cur_Svngs_Inp)/DATEDIF(TODAY(), Trgt_Svngs_Date_Inp, "M")</f>
+        <v>572.67441860465112</v>
+      </c>
+      <c r="E10" s="47"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="25"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="30">
-        <f ca="1">D10/'Budget Calc'!D4</f>
-        <v>9.5578975047400261E-2</v>
-      </c>
-      <c r="E12" s="30"/>
-    </row>
-    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="29"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="48">
+        <f ca="1">IF(Tot_Mnthly_Inc_Inp&gt;0, Mnthly_Svngs_Needed_Out/Tot_Mnthly_Inc_Inp, "0 or less Total Monthly Income")</f>
+        <v>7.5292455772370648E-2</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="46">
+        <f>Bdgt_Calc_Out</f>
+        <v>1938</v>
+      </c>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="29"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B10:C10"/>
@@ -1108,64 +1693,97 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10" xr:uid="{8FD41BBB-9977-4F65-BD8D-117F454F23FA}">
+      <formula1>Bgt_Without_Savngs</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2057" r:id="rId4" name="Scroll Bar 9">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2058" r:id="rId5" name="Scroll Bar 10">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769DB53D-0AAC-4644-8617-4C476A4CF40D}">
-  <dimension ref="A1:B4"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63738CA-DCA2-4031-A665-6A49C51F0E5A}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2">
+        <v>53</v>
       </c>
       <c r="B2">
-        <v>4280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>3026</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>300</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1173,131 +1791,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E94264-42BD-47F2-AF08-57474E473BB2}">
-  <dimension ref="A1:B14"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A532210-BA0B-4A66-B604-B320D8DFFF95}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1305,13 +1824,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B74DB-4983-42F8-ADCD-041BE9523AEC}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1478,11 +1997,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224E40E2-FE54-4FAF-9537-95269AC4597A}">
   <dimension ref="A1:D2327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>

</xml_diff>

<commit_message>
Only Data Viz notes updated. Budget updates coming in few hours.
</commit_message>
<xml_diff>
--- a/Excel_Project/BUDGET_PROJECT.xlsx
+++ b/Excel_Project/BUDGET_PROJECT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Excel_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE79B27E-8913-4604-A037-FE8956113531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA1FE39-1EC5-41F0-AA51-6EE6C974E93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Calc" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4702" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4703" uniqueCount="106">
   <si>
     <t>BUDGET AND EXPENSE SUMMARY</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Savings Target Date</t>
+  </si>
+  <si>
+    <t>DAILY BUDGET</t>
   </si>
 </sst>
 </file>
@@ -705,83 +708,17 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -803,20 +740,92 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="14" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -923,7 +932,7 @@
                   <a14:compatExt spid="_x0000_s2058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E77CB55-1F19-4111-8037-55679FB2BFBD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1216,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,80 +1241,98 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="45">
+      <c r="C4" s="30"/>
+      <c r="D4" s="23">
         <f>SUM('Monthyl Incomes'!B:B)</f>
         <v>7606</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="21"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="45">
+      <c r="C6" s="30"/>
+      <c r="D6" s="23">
         <f>SUM('Monthly Expenses'!B:B)</f>
         <v>5668</v>
       </c>
-      <c r="E6" s="41"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="46">
+      <c r="C8" s="34"/>
+      <c r="D8" s="24">
         <f>IF(Bgt_Without_Svngs_Inp="No", (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp), (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp-Cur_Svngs_Inp))</f>
         <v>1938</v>
       </c>
-      <c r="E8" s="42"/>
-    </row>
-    <row r="9" spans="2:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="44"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="24">
+        <f>Bdgt_Calc_Out/30</f>
+        <v>64.599999999999994</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1500,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383BEB5-BBAF-43B5-BACD-CE422F08E9FE}">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1514,169 +1541,162 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="36"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="50">
+      <c r="C4" s="30"/>
+      <c r="D4" s="41">
         <f>'Savings Goal Linked Cells (H)'!A2*1000</f>
         <v>53000</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="34"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="21"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="34"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="51">
+      <c r="C6" s="30"/>
+      <c r="D6" s="45">
         <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())+'Savings Goal Linked Cells (H)'!B2, DAY(TODAY()))</f>
-        <v>47208</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="34"/>
+        <v>47209</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="22"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="49">
+      <c r="C8" s="30"/>
+      <c r="D8" s="46">
         <v>3750</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="34"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="23"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="34"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="47">
+      <c r="C10" s="34"/>
+      <c r="D10" s="44">
         <f ca="1">(Svngs_Goal_Inp-Cur_Svngs_Inp)/DATEDIF(TODAY(), Trgt_Svngs_Date_Inp, "M")</f>
         <v>572.67441860465112</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="33" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="25"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="34"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="48">
+      <c r="C12" s="34"/>
+      <c r="D12" s="53">
         <f ca="1">IF(Tot_Mnthly_Inc_Inp&gt;0, Mnthly_Svngs_Needed_Out/Tot_Mnthly_Inc_Inp, "0 or less Total Monthly Income")</f>
         <v>7.5292455772370648E-2</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="33" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="24">
         <f>Bdgt_Calc_Out</f>
         <v>1938</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B10:C10"/>
@@ -1693,6 +1713,13 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10" xr:uid="{8FD41BBB-9977-4F65-BD8D-117F454F23FA}">

</xml_diff>

<commit_message>
Budget Project update with Income, Expense and Spending Summary charts viz.
</commit_message>
<xml_diff>
--- a/Excel_Project/BUDGET_PROJECT.xlsx
+++ b/Excel_Project/BUDGET_PROJECT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\Excel_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA1FE39-1EC5-41F0-AA51-6EE6C974E93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B471D6C0-D988-4A89-B6BA-FE385CC367D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Calc" sheetId="1" r:id="rId1"/>
@@ -740,6 +740,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -758,39 +776,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -805,6 +790,12 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -827,6 +818,15 @@
     <xf numFmtId="10" fontId="9" fillId="6" borderId="7" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -836,8 +836,45 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE5AF37"/>
+      <color rgb="FFCC0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -849,6 +886,3210 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Income</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> v/s Expense</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total Monthly Income</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budget Calc'!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7606</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6E54-4975-8F79-1024E091EFA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Total Monthly Expense</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Budget Calc'!$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6E54-4975-8F79-1024E091EFA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="529921992"/>
+        <c:axId val="529929208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="529921992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="529929208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="529929208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>MONTHLY INCOME /</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t> EXPENSE AMOUNT </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1400">
+                  <a:solidFill>
+                    <a:srgbClr val="E5AF37"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529921992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Monthly Expense</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Monthly Expense Amount</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Monthly Expenses'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Rent/Mortgage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cell phone</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Groceries</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Car payment</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Auto repair/maintenance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Auto Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Entertainment</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dining</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Phone/Cable</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Miscellaneous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Monthly Expenses'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3891-4C9A-B0D1-20D0CC9EAEB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="553177136"/>
+        <c:axId val="553180744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="553177136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553180744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="553180744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>Monthly expense amount </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E5AF37"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553177136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spending</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Summary by Category</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Money Spent</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Spending Summary'!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Mortgage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gas/Automotive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dining</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Merchandise</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Other</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Other Services</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lodging</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Airfare</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Professional Services</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Entertainment</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Other Travel</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Phone/Cable</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Payment/Credit</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Health Care</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Internet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Spending Summary'!$B$2:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>43820</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12071.640000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31147.119999999977</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51422.080000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4222.7400000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4224.3999999999978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3420.88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3178.6599999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6332.4900000000016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8687.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>695.44999999999993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2566.34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4381.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288.96000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1096.2099999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5DD-4021-A3B0-317F0618B703}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="434461224"/>
+        <c:axId val="434457944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="434461224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434457944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="434457944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>spending amount </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="E5AF37"/>
+                    </a:solidFill>
+                    <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  </a:rPr>
+                  <a:t>($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr lang="en-CA" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="E5AF37"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434461224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="'Savings Goal Linked Cells (H)'!$A$2" horiz="1" max="100" page="10" val="53"/>
 </file>
@@ -858,6 +4099,83 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF210E31-A223-4EF9-9208-C39D567E6F67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CC29416-B778-47E8-B48C-BD15FFFF5269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -959,6 +4277,47 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A3A162-707D-4E35-A599-4ABA5D5BF296}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1227,8 +4586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,24 +4600,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="23">
         <f>SUM('Monthyl Incomes'!B:B)</f>
         <v>7606</v>
@@ -1266,16 +4625,16 @@
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="16"/>
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="23">
         <f>SUM('Monthly Expenses'!B:B)</f>
         <v>5668</v>
@@ -1283,16 +4642,16 @@
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="16"/>
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="24">
         <f>IF(Bgt_Without_Svngs_Inp="No", (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp), (Tot_Mnthly_Inc_Inp-Tot_Mnthly_Expns_Inp-Cur_Svngs_Inp))</f>
         <v>1938</v>
@@ -1306,10 +4665,10 @@
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="24">
         <f>Bdgt_Calc_Out/30</f>
         <v>64.599999999999994</v>
@@ -1317,8 +4676,8 @@
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="2:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
     </row>
@@ -1334,8 +4693,14 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
+  <conditionalFormatting sqref="D8 D10">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1528,7 +4893,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,111 +4906,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="41">
+      <c r="C4" s="36"/>
+      <c r="D4" s="53">
         <f>'Savings Goal Linked Cells (H)'!A2*1000</f>
         <v>53000</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="45">
+      <c r="C6" s="36"/>
+      <c r="D6" s="40">
         <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())+'Savings Goal Linked Cells (H)'!B2, DAY(TODAY()))</f>
         <v>47209</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="46">
+      <c r="C8" s="36"/>
+      <c r="D8" s="41">
         <v>3750</v>
       </c>
-      <c r="E8" s="46"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="49"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="44">
+      <c r="C10" s="28"/>
+      <c r="D10" s="39">
         <f ca="1">(Svngs_Goal_Inp-Cur_Svngs_Inp)/DATEDIF(TODAY(), Trgt_Svngs_Date_Inp, "M")</f>
         <v>572.67441860465112</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="8"/>
       <c r="G10" s="11" t="s">
         <v>98</v>
@@ -1656,25 +5021,25 @@
       <c r="I10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="53">
+      <c r="C12" s="28"/>
+      <c r="D12" s="50">
         <f ca="1">IF(Tot_Mnthly_Inc_Inp&gt;0, Mnthly_Svngs_Needed_Out/Tot_Mnthly_Inc_Inp, "0 or less Total Monthly Income")</f>
         <v>7.5292455772370648E-2</v>
       </c>
-      <c r="E12" s="53"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="8"/>
       <c r="G12" s="11" t="s">
         <v>102</v>
@@ -1686,10 +5051,10 @@
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1697,6 +5062,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B10:C10"/>
@@ -1713,14 +5085,12 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10" xr:uid="{8FD41BBB-9977-4F65-BD8D-117F454F23FA}">
       <formula1>Bgt_Without_Savngs</formula1>
@@ -1855,9 +5225,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B74DB-4983-42F8-ADCD-041BE9523AEC}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,6 +5391,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>